<commit_message>
one more try LR3/1
</commit_message>
<xml_diff>
--- a/LR3/table_1_108.xlsx
+++ b/LR3/table_1_108.xlsx
@@ -1952,7 +1952,7 @@
         <v>54</v>
       </c>
       <c r="D35" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">A$1*0.55</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">$D$3/2</f>
         <v>59.4</v>
       </c>
       <c r="E35" s="2" t="n">
@@ -1997,7 +1997,7 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">A$1*1.1/2</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">$D$3/2</f>
         <v>59.4</v>
       </c>
       <c r="E36" s="2" t="n">
@@ -2042,7 +2042,7 @@
         <v>53</v>
       </c>
       <c r="D37" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">A$1*1.1/2</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">$D$3/2</f>
         <v>59.4</v>
       </c>
       <c r="E37" s="2" t="n">
@@ -2087,7 +2087,7 @@
         <v>52.5</v>
       </c>
       <c r="D38" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D37</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">$D$3/2</f>
         <v>59.4</v>
       </c>
       <c r="E38" s="2" t="n">
@@ -2145,7 +2145,7 @@
         <v>49</v>
       </c>
       <c r="C42" s="4" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">MAX(H3, H38)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">MAX(H3:H38)</f>
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
one more try2 LR3/1
</commit_message>
<xml_diff>
--- a/LR3/table_1_108.xlsx
+++ b/LR3/table_1_108.xlsx
@@ -162,7 +162,7 @@
     <t>Максимальный срок просрочки, дней</t>
   </si>
   <si>
-    <t>Максимальная сумма к оплате, руб.</t>
+    <t>Максимальная сумма, руб.</t>
   </si>
 </sst>
 </file>
@@ -1518,7 +1518,7 @@
         <v>44827</v>
       </c>
       <c r="H25" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(SUM(G25, -F25)&lt;0, 0, SUM(G25, -F25))</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G25&lt;=F25, 0, G25-F25)</f>
         <v>14</v>
       </c>
       <c r="I25" s="4" t="n">
@@ -1563,7 +1563,7 @@
         <v>44828</v>
       </c>
       <c r="H26" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(SUM(G26, -F26)&lt;0, 0, SUM(G26, -F26))</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G26&lt;=F26, 0, G26-F26)</f>
         <v>15</v>
       </c>
       <c r="I26" s="4" t="n">
@@ -1608,7 +1608,7 @@
         <v>44829</v>
       </c>
       <c r="H27" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(SUM(G27, -F27)&lt;0, 0, SUM(G27, -F27))</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G27&lt;=F27, 0, G27-F27)</f>
         <v>16</v>
       </c>
       <c r="I27" s="4" t="n">
@@ -1653,7 +1653,7 @@
         <v>44830</v>
       </c>
       <c r="H28" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(SUM(G28, -F28)&lt;0, 0, SUM(G28, -F28))</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G28&lt;=F28, 0, G28-F28)</f>
         <v>17</v>
       </c>
       <c r="I28" s="4" t="n">
@@ -1698,7 +1698,7 @@
         <v>44831</v>
       </c>
       <c r="H29" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(SUM(G29, -F29)&lt;0, 0, SUM(G29, -F29))</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G29&lt;=F29, 0, G29-F29)</f>
         <v>18</v>
       </c>
       <c r="I29" s="4" t="n">
@@ -1743,7 +1743,7 @@
         <v>44832</v>
       </c>
       <c r="H30" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(SUM(G30, -F30)&lt;0, 0, SUM(G30, -F30))</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G30&lt;=F30, 0, G30-F30)</f>
         <v>19</v>
       </c>
       <c r="I30" s="4" t="n">
@@ -1788,7 +1788,7 @@
         <v>44833</v>
       </c>
       <c r="H31" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(SUM(G31, -F31)&lt;0, 0, SUM(G31, -F31))</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G31&lt;=F31, 0, G31-F31)</f>
         <v>20</v>
       </c>
       <c r="I31" s="4" t="n">
@@ -1833,7 +1833,7 @@
         <v>44834</v>
       </c>
       <c r="H32" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(SUM(G32, -F32)&lt;0, 0, SUM(G32, -F32))</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G32&lt;=F32, 0, G32-F32)</f>
         <v>21</v>
       </c>
       <c r="I32" s="4" t="n">
@@ -1878,7 +1878,7 @@
         <v>44835</v>
       </c>
       <c r="H33" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(SUM(G33, -F33)&lt;0, 0, SUM(G33, -F33))</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G33&lt;=F33, 0, G33-F33)</f>
         <v>22</v>
       </c>
       <c r="I33" s="4" t="n">
@@ -1923,7 +1923,7 @@
         <v>44836</v>
       </c>
       <c r="H34" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(SUM(G34, -F34)&lt;0, 0, SUM(G34, -F34))</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G34&lt;=F34, 0, G34-F34)</f>
         <v>23</v>
       </c>
       <c r="I34" s="4" t="n">
@@ -1952,7 +1952,7 @@
         <v>54</v>
       </c>
       <c r="D35" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">$D$3/2</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">A1*1.1/2</f>
         <v>59.4</v>
       </c>
       <c r="E35" s="2" t="n">
@@ -1968,7 +1968,7 @@
         <v>44837</v>
       </c>
       <c r="H35" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(SUM(G35, -F35)&lt;0, 0, SUM(G35, -F35))</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G35&lt;=F35, 0, G35-F35)</f>
         <v>24</v>
       </c>
       <c r="I35" s="4" t="n">
@@ -1997,7 +1997,7 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">$D$3/2</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D35</f>
         <v>59.4</v>
       </c>
       <c r="E36" s="2" t="n">
@@ -2013,7 +2013,7 @@
         <v>44838</v>
       </c>
       <c r="H36" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(SUM(G36, -F36)&lt;0, 0, SUM(G36, -F36))</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G36&lt;=F36, 0, G36-F36)</f>
         <v>25</v>
       </c>
       <c r="I36" s="4" t="n">
@@ -2042,7 +2042,7 @@
         <v>53</v>
       </c>
       <c r="D37" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">$D$3/2</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D36</f>
         <v>59.4</v>
       </c>
       <c r="E37" s="2" t="n">
@@ -2058,7 +2058,7 @@
         <v>44839</v>
       </c>
       <c r="H37" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(SUM(G37, -F37)&lt;0, 0, SUM(G37, -F37))</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G37&lt;=F37, 0, G37-F37)</f>
         <v>26</v>
       </c>
       <c r="I37" s="4" t="n">
@@ -2087,7 +2087,7 @@
         <v>52.5</v>
       </c>
       <c r="D38" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">$D$3/2</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D37</f>
         <v>59.4</v>
       </c>
       <c r="E38" s="2" t="n">
@@ -2103,7 +2103,7 @@
         <v>44840</v>
       </c>
       <c r="H38" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(SUM(G38, -F38)&lt;0, 0, SUM(G38, -F38))</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G38&lt;=F38, 0, G38-F38)</f>
         <v>27</v>
       </c>
       <c r="I38" s="4" t="n">
@@ -2154,7 +2154,7 @@
         <v>50</v>
       </c>
       <c r="C43" s="4" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">MAX(K3, K38)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">MAX(K3:K38)</f>
         <v>8316</v>
       </c>
     </row>

</xml_diff>

<commit_message>
one more try3 LR3/1
</commit_message>
<xml_diff>
--- a/LR3/table_1_108.xlsx
+++ b/LR3/table_1_108.xlsx
@@ -147,10 +147,10 @@
     <t>Шаймарданова</t>
   </si>
   <si>
+    <t>Кузин</t>
+  </si>
+  <si>
     <t>Куропаткин 1</t>
-  </si>
-  <si>
-    <t>Куропаткин 2</t>
   </si>
   <si>
     <t>Общая сумма, руб.</t>
@@ -515,7 +515,7 @@
         <v>70</v>
       </c>
       <c r="D3" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">A1*1.1</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E3" s="2" t="n">
@@ -529,7 +529,7 @@
         <v>44805</v>
       </c>
       <c r="H3" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G3&lt;=F3, 0, G3-F3)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F3&gt;=G3, 0, G3-F3)</f>
         <v>0</v>
       </c>
       <c r="I3" s="4" t="n">
@@ -557,7 +557,7 @@
         <v>69.5</v>
       </c>
       <c r="D4" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D3</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E4" s="2" t="n">
@@ -573,7 +573,7 @@
         <v>44806</v>
       </c>
       <c r="H4" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G4&lt;=F4, 0, G4-F4)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F4&gt;=G4, 0, G4-F4)</f>
         <v>0</v>
       </c>
       <c r="I4" s="4" t="n">
@@ -602,7 +602,7 @@
         <v>69</v>
       </c>
       <c r="D5" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D4</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E5" s="2" t="n">
@@ -618,7 +618,7 @@
         <v>44807</v>
       </c>
       <c r="H5" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G5&lt;=F5, 0, G5-F5)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F5&gt;=G5, 0, G5-F5)</f>
         <v>0</v>
       </c>
       <c r="I5" s="4" t="n">
@@ -647,7 +647,7 @@
         <v>68.5</v>
       </c>
       <c r="D6" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D5</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E6" s="2" t="n">
@@ -663,7 +663,7 @@
         <v>44808</v>
       </c>
       <c r="H6" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G6&lt;=F6, 0, G6-F6)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F6&gt;=G6, 0, G6-F6)</f>
         <v>0</v>
       </c>
       <c r="I6" s="4" t="n">
@@ -692,7 +692,7 @@
         <v>68</v>
       </c>
       <c r="D7" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D6</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E7" s="2" t="n">
@@ -708,7 +708,7 @@
         <v>44809</v>
       </c>
       <c r="H7" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G7&lt;=F7, 0, G7-F7)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F7&gt;=G7, 0, G7-F7)</f>
         <v>0</v>
       </c>
       <c r="I7" s="4" t="n">
@@ -737,7 +737,7 @@
         <v>67.5</v>
       </c>
       <c r="D8" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D7</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E8" s="2" t="n">
@@ -753,7 +753,7 @@
         <v>44810</v>
       </c>
       <c r="H8" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G8&lt;=F8, 0, G8-F8)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F8&gt;=G8, 0, G8-F8)</f>
         <v>0</v>
       </c>
       <c r="I8" s="4" t="n">
@@ -782,7 +782,7 @@
         <v>67</v>
       </c>
       <c r="D9" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D8</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E9" s="2" t="n">
@@ -798,7 +798,7 @@
         <v>44811</v>
       </c>
       <c r="H9" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G9&lt;=F9, 0, G9-F9)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F9&gt;=G9, 0, G9-F9)</f>
         <v>0</v>
       </c>
       <c r="I9" s="4" t="n">
@@ -827,7 +827,7 @@
         <v>66.5</v>
       </c>
       <c r="D10" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D9</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E10" s="2" t="n">
@@ -843,7 +843,7 @@
         <v>44812</v>
       </c>
       <c r="H10" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G10&lt;=F10, 0, G10-F10)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F10&gt;=G10, 0, G10-F10)</f>
         <v>0</v>
       </c>
       <c r="I10" s="4" t="n">
@@ -872,7 +872,7 @@
         <v>66</v>
       </c>
       <c r="D11" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D10</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E11" s="2" t="n">
@@ -888,7 +888,7 @@
         <v>44813</v>
       </c>
       <c r="H11" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G11&lt;=F11, 0, G11-F11)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F11&gt;=G11, 0, G11-F11)</f>
         <v>0</v>
       </c>
       <c r="I11" s="4" t="n">
@@ -917,7 +917,7 @@
         <v>65.5</v>
       </c>
       <c r="D12" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D11</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E12" s="2" t="n">
@@ -933,7 +933,7 @@
         <v>44814</v>
       </c>
       <c r="H12" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G12&lt;=F12, 0, G12-F12)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F12&gt;=G12, 0, G12-F12)</f>
         <v>1</v>
       </c>
       <c r="I12" s="4" t="n">
@@ -962,7 +962,7 @@
         <v>65</v>
       </c>
       <c r="D13" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D12</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E13" s="2" t="n">
@@ -978,7 +978,7 @@
         <v>44815</v>
       </c>
       <c r="H13" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G13&lt;=F13, 0, G13-F13)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F13&gt;=G13, 0, G13-F13)</f>
         <v>2</v>
       </c>
       <c r="I13" s="4" t="n">
@@ -1007,7 +1007,7 @@
         <v>64.5</v>
       </c>
       <c r="D14" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D13</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E14" s="2" t="n">
@@ -1023,7 +1023,7 @@
         <v>44816</v>
       </c>
       <c r="H14" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G14&lt;=F14, 0, G14-F14)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F14&gt;=G14, 0, G14-F14)</f>
         <v>3</v>
       </c>
       <c r="I14" s="4" t="n">
@@ -1052,7 +1052,7 @@
         <v>64</v>
       </c>
       <c r="D15" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D14</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E15" s="2" t="n">
@@ -1068,7 +1068,7 @@
         <v>44817</v>
       </c>
       <c r="H15" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G15&lt;=F15, 0, G15-F15)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F15&gt;=G15, 0, G15-F15)</f>
         <v>4</v>
       </c>
       <c r="I15" s="4" t="n">
@@ -1097,7 +1097,7 @@
         <v>63.5</v>
       </c>
       <c r="D16" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D15</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E16" s="2" t="n">
@@ -1113,7 +1113,7 @@
         <v>44818</v>
       </c>
       <c r="H16" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G16&lt;=F16, 0, G16-F16)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F16&gt;=G16, 0, G16-F16)</f>
         <v>5</v>
       </c>
       <c r="I16" s="4" t="n">
@@ -1142,7 +1142,7 @@
         <v>63</v>
       </c>
       <c r="D17" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D16</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E17" s="2" t="n">
@@ -1158,7 +1158,7 @@
         <v>44819</v>
       </c>
       <c r="H17" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G17&lt;=F17, 0, G17-F17)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F17&gt;=G17, 0, G17-F17)</f>
         <v>6</v>
       </c>
       <c r="I17" s="4" t="n">
@@ -1187,7 +1187,7 @@
         <v>62.5</v>
       </c>
       <c r="D18" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D17</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E18" s="2" t="n">
@@ -1203,7 +1203,7 @@
         <v>44820</v>
       </c>
       <c r="H18" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G18&lt;=F18, 0, G18-F18)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F18&gt;=G18, 0, G18-F18)</f>
         <v>7</v>
       </c>
       <c r="I18" s="4" t="n">
@@ -1232,7 +1232,7 @@
         <v>62</v>
       </c>
       <c r="D19" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D18</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E19" s="2" t="n">
@@ -1248,7 +1248,7 @@
         <v>44821</v>
       </c>
       <c r="H19" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G19&lt;=F19, 0, G19-F19)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F19&gt;=G19, 0, G19-F19)</f>
         <v>8</v>
       </c>
       <c r="I19" s="4" t="n">
@@ -1277,7 +1277,7 @@
         <v>61.5</v>
       </c>
       <c r="D20" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D19</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E20" s="2" t="n">
@@ -1293,7 +1293,7 @@
         <v>44822</v>
       </c>
       <c r="H20" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G20&lt;=F20, 0, G20-F20)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F20&gt;=G20, 0, G20-F20)</f>
         <v>9</v>
       </c>
       <c r="I20" s="4" t="n">
@@ -1322,7 +1322,7 @@
         <v>61</v>
       </c>
       <c r="D21" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D20</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E21" s="2" t="n">
@@ -1338,7 +1338,7 @@
         <v>44823</v>
       </c>
       <c r="H21" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G21&lt;=F21, 0, G21-F21)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F21&gt;=G21, 0, G21-F21)</f>
         <v>10</v>
       </c>
       <c r="I21" s="4" t="n">
@@ -1367,7 +1367,7 @@
         <v>60.5</v>
       </c>
       <c r="D22" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D21</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E22" s="2" t="n">
@@ -1383,7 +1383,7 @@
         <v>44824</v>
       </c>
       <c r="H22" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G22&lt;=F22, 0, G22-F22)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F22&gt;=G22, 0, G22-F22)</f>
         <v>11</v>
       </c>
       <c r="I22" s="4" t="n">
@@ -1412,7 +1412,7 @@
         <v>60</v>
       </c>
       <c r="D23" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D22</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E23" s="2" t="n">
@@ -1428,7 +1428,7 @@
         <v>44825</v>
       </c>
       <c r="H23" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G23&lt;=F23, 0, G23-F23)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F23&gt;=G23, 0, G23-F23)</f>
         <v>12</v>
       </c>
       <c r="I23" s="4" t="n">
@@ -1457,7 +1457,7 @@
         <v>59.5</v>
       </c>
       <c r="D24" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D23</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E24" s="2" t="n">
@@ -1473,7 +1473,7 @@
         <v>44826</v>
       </c>
       <c r="H24" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G24&lt;=F24, 0, G24-F24)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F24&gt;=G24, 0, G24-F24)</f>
         <v>13</v>
       </c>
       <c r="I24" s="4" t="n">
@@ -1502,7 +1502,7 @@
         <v>59</v>
       </c>
       <c r="D25" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D24</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E25" s="2" t="n">
@@ -1518,7 +1518,7 @@
         <v>44827</v>
       </c>
       <c r="H25" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G25&lt;=F25, 0, G25-F25)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F25&gt;=G25, 0, G25-F25)</f>
         <v>14</v>
       </c>
       <c r="I25" s="4" t="n">
@@ -1547,7 +1547,7 @@
         <v>58.5</v>
       </c>
       <c r="D26" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D25</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E26" s="2" t="n">
@@ -1563,7 +1563,7 @@
         <v>44828</v>
       </c>
       <c r="H26" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G26&lt;=F26, 0, G26-F26)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F26&gt;=G26, 0, G26-F26)</f>
         <v>15</v>
       </c>
       <c r="I26" s="4" t="n">
@@ -1592,7 +1592,7 @@
         <v>58</v>
       </c>
       <c r="D27" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D26</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E27" s="2" t="n">
@@ -1608,7 +1608,7 @@
         <v>44829</v>
       </c>
       <c r="H27" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G27&lt;=F27, 0, G27-F27)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F27&gt;=G27, 0, G27-F27)</f>
         <v>16</v>
       </c>
       <c r="I27" s="4" t="n">
@@ -1637,7 +1637,7 @@
         <v>57.5</v>
       </c>
       <c r="D28" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D27</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E28" s="2" t="n">
@@ -1653,7 +1653,7 @@
         <v>44830</v>
       </c>
       <c r="H28" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G28&lt;=F28, 0, G28-F28)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F28&gt;=G28, 0, G28-F28)</f>
         <v>17</v>
       </c>
       <c r="I28" s="4" t="n">
@@ -1682,7 +1682,7 @@
         <v>57</v>
       </c>
       <c r="D29" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D28</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E29" s="2" t="n">
@@ -1698,7 +1698,7 @@
         <v>44831</v>
       </c>
       <c r="H29" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G29&lt;=F29, 0, G29-F29)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F29&gt;=G29, 0, G29-F29)</f>
         <v>18</v>
       </c>
       <c r="I29" s="4" t="n">
@@ -1727,7 +1727,7 @@
         <v>56.5</v>
       </c>
       <c r="D30" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D29</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E30" s="2" t="n">
@@ -1743,7 +1743,7 @@
         <v>44832</v>
       </c>
       <c r="H30" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G30&lt;=F30, 0, G30-F30)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F30&gt;=G30, 0, G30-F30)</f>
         <v>19</v>
       </c>
       <c r="I30" s="4" t="n">
@@ -1772,7 +1772,7 @@
         <v>56</v>
       </c>
       <c r="D31" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D30</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E31" s="2" t="n">
@@ -1788,7 +1788,7 @@
         <v>44833</v>
       </c>
       <c r="H31" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G31&lt;=F31, 0, G31-F31)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F31&gt;=G31, 0, G31-F31)</f>
         <v>20</v>
       </c>
       <c r="I31" s="4" t="n">
@@ -1817,7 +1817,7 @@
         <v>55.5</v>
       </c>
       <c r="D32" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D31</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E32" s="2" t="n">
@@ -1833,7 +1833,7 @@
         <v>44834</v>
       </c>
       <c r="H32" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G32&lt;=F32, 0, G32-F32)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F32&gt;=G32, 0, G32-F32)</f>
         <v>21</v>
       </c>
       <c r="I32" s="4" t="n">
@@ -1862,7 +1862,7 @@
         <v>55</v>
       </c>
       <c r="D33" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D32</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E33" s="2" t="n">
@@ -1878,7 +1878,7 @@
         <v>44835</v>
       </c>
       <c r="H33" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G33&lt;=F33, 0, G33-F33)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F33&gt;=G33, 0, G33-F33)</f>
         <v>22</v>
       </c>
       <c r="I33" s="4" t="n">
@@ -1907,7 +1907,7 @@
         <v>54.5</v>
       </c>
       <c r="D34" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D33</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">1.1*$A$1</f>
         <v>118.8</v>
       </c>
       <c r="E34" s="2" t="n">
@@ -1923,7 +1923,7 @@
         <v>44836</v>
       </c>
       <c r="H34" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G34&lt;=F34, 0, G34-F34)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F34&gt;=G34, 0, G34-F34)</f>
         <v>23</v>
       </c>
       <c r="I34" s="4" t="n">
@@ -1952,7 +1952,7 @@
         <v>54</v>
       </c>
       <c r="D35" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">A1*1.1/2</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">$D$34/2</f>
         <v>59.4</v>
       </c>
       <c r="E35" s="2" t="n">
@@ -1968,7 +1968,7 @@
         <v>44837</v>
       </c>
       <c r="H35" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G35&lt;=F35, 0, G35-F35)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F35&gt;=G35, 0, G35-F35)</f>
         <v>24</v>
       </c>
       <c r="I35" s="4" t="n">
@@ -1997,7 +1997,7 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D35</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">$D$34/2</f>
         <v>59.4</v>
       </c>
       <c r="E36" s="2" t="n">
@@ -2013,7 +2013,7 @@
         <v>44838</v>
       </c>
       <c r="H36" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G36&lt;=F36, 0, G36-F36)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F36&gt;=G36, 0, G36-F36)</f>
         <v>25</v>
       </c>
       <c r="I36" s="4" t="n">
@@ -2042,7 +2042,7 @@
         <v>53</v>
       </c>
       <c r="D37" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D36</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">$D$34/2</f>
         <v>59.4</v>
       </c>
       <c r="E37" s="2" t="n">
@@ -2058,7 +2058,7 @@
         <v>44839</v>
       </c>
       <c r="H37" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G37&lt;=F37, 0, G37-F37)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F37&gt;=G37, 0, G37-F37)</f>
         <v>26</v>
       </c>
       <c r="I37" s="4" t="n">
@@ -2087,7 +2087,7 @@
         <v>52.5</v>
       </c>
       <c r="D38" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">D37</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">$D$34/2</f>
         <v>59.4</v>
       </c>
       <c r="E38" s="2" t="n">
@@ -2103,7 +2103,7 @@
         <v>44840</v>
       </c>
       <c r="H38" s="2" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(G38&lt;=F38, 0, G38-F38)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">IF(F38&gt;=G38, 0, G38-F38)</f>
         <v>27</v>
       </c>
       <c r="I38" s="4" t="n">
@@ -2154,7 +2154,7 @@
         <v>50</v>
       </c>
       <c r="C43" s="4" t="n">
-        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">MAX(K3:K38)</f>
+        <f aca="false" ca="false" dt2D="false" dtr="false" t="normal">MAX(K3, K38)</f>
         <v>8316</v>
       </c>
     </row>

</xml_diff>